<commit_message>
agregate functions and remade gherkin
</commit_message>
<xml_diff>
--- a/src/main/resources/excel/FlujosMCSS.xlsx
+++ b/src/main/resources/excel/FlujosMCSS.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="41">
   <si>
     <t>TC1</t>
   </si>
@@ -153,7 +153,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="00"/>
   </numFmts>
-  <fonts count="105" x14ac:knownFonts="1">
+  <fonts count="137" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -190,6 +190,134 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
     </font>
     <font>
       <name val="Calibri"/>
@@ -613,7 +741,7 @@
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="111">
+  <cellXfs count="143">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -734,7 +862,39 @@
     <xf applyFont="true" borderId="0" fillId="0" fontId="101" numFmtId="0" xfId="0"/>
     <xf applyFont="true" borderId="0" fillId="0" fontId="102" numFmtId="0" xfId="0"/>
     <xf applyFont="true" borderId="0" fillId="0" fontId="103" numFmtId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="104" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="104" numFmtId="0" xfId="0"/>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="105" numFmtId="0" xfId="0"/>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="106" numFmtId="0" xfId="0"/>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="107" numFmtId="0" xfId="0"/>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="108" numFmtId="0" xfId="0"/>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="109" numFmtId="0" xfId="0"/>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="110" numFmtId="0" xfId="0"/>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="111" numFmtId="0" xfId="0"/>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="112" numFmtId="0" xfId="0"/>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="113" numFmtId="0" xfId="0"/>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="114" numFmtId="0" xfId="0"/>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="115" numFmtId="0" xfId="0"/>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="116" numFmtId="0" xfId="0"/>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="117" numFmtId="0" xfId="0"/>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="118" numFmtId="0" xfId="0"/>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="119" numFmtId="0" xfId="0"/>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="120" numFmtId="0" xfId="0"/>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="121" numFmtId="0" xfId="0"/>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="122" numFmtId="0" xfId="0"/>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="123" numFmtId="0" xfId="0"/>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="124" numFmtId="0" xfId="0"/>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="125" numFmtId="0" xfId="0"/>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="126" numFmtId="0" xfId="0"/>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="127" numFmtId="0" xfId="0"/>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="128" numFmtId="0" xfId="0"/>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="129" numFmtId="0" xfId="0"/>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="130" numFmtId="0" xfId="0"/>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="131" numFmtId="0" xfId="0"/>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="132" numFmtId="0" xfId="0"/>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="133" numFmtId="0" xfId="0"/>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="134" numFmtId="0" xfId="0"/>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="135" numFmtId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="136" fillId="0" borderId="0" xfId="0" applyFont="true"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle builtinId="8" name="Hipervínculo" xfId="1"/>

</xml_diff>